<commit_message>
few things (see description)
added pokemon type enum and data
fixed errors with widgets not getting correct data from attacks
removed old functions from game state and game mode
added new fns to battle manager
Next steps: in the "calculate damage" function of battle manager, add the type effectiveness to the modifier at the end, multiply the modifer with the preliminary value to get final dmg value, then we need to apply the dmg to the defending pokemon, and finally we need to remove this logic from the game mode
</commit_message>
<xml_diff>
--- a/Content/Pokemon/_Data/pokemon-data.xlsx
+++ b/Content/Pokemon/_Data/pokemon-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shivi\Desktop\PokemonRemake\Content\Pokemon\_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unreal\PokemonRemake\Content\Pokemon\_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{883F3EAA-3632-4540-8B3A-4AF5BA07B133}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC80D14-7E41-4224-ACDF-763D9A0DFDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="46080" windowHeight="22020" xr2:uid="{85508672-8284-4726-8A97-6AD16808DEE1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{85508672-8284-4726-8A97-6AD16808DEE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -49,6 +49,30 @@
   </si>
   <si>
     <t>Birb</t>
+  </si>
+  <si>
+    <t>Type2</t>
+  </si>
+  <si>
+    <t>Type1</t>
+  </si>
+  <si>
+    <t>Birb-H</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Flying</t>
+  </si>
+  <si>
+    <t>Ice</t>
   </si>
 </sst>
 </file>
@@ -104,9 +128,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -144,7 +168,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -250,7 +274,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -392,7 +416,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -400,20 +424,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF18A8C-F114-4A2B-B8C1-A078FA5C0837}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -427,45 +451,89 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="D2">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E2">
+        <v>43</v>
+      </c>
+      <c r="F2">
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
         <v>45</v>
       </c>
-      <c r="F2">
-        <v>80</v>
+      <c r="E3">
+        <v>40</v>
+      </c>
+      <c r="F3">
+        <v>56</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>80</v>
-      </c>
-      <c r="D3">
-        <v>80</v>
-      </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-      <c r="F3">
-        <v>120</v>
+      <c r="C4">
+        <v>56</v>
+      </c>
+      <c r="D4">
+        <v>45</v>
+      </c>
+      <c r="E4">
+        <v>40</v>
+      </c>
+      <c r="F4">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>